<commit_message>
Update ETRX ECU excel documents
</commit_message>
<xml_diff>
--- a/ETRX_FECU/HW_FECU.xlsx
+++ b/ETRX_FECU/HW_FECU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9068b3d81be815ab/download/New/download/Documentos/GitHub/ADCAN/ETRX_FECU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4D2F04E46CFB4ACB3E201215D3DB9A693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E93ABF2E-BF31-4A8E-9947-D0D2F39E8EEA}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_AD4D2F04E46CFB4ACB3E201215D3DB9A693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A222F48-7E7F-4AF4-BD4B-269E721E1390}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="3150" windowWidth="18780" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Sensor</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Vcc (v)</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
@@ -117,12 +114,33 @@
   </si>
   <si>
     <t>Conn pins</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>Tyre_temperatuae</t>
+  </si>
+  <si>
+    <t>MLX90641</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QEUmVspiburSFoTysupAeOcM1dWjx5MP/view</t>
+  </si>
+  <si>
+    <t>P (W)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -230,12 +248,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -245,6 +285,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -526,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,14 +580,15 @@
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="97.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="97.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -553,147 +597,156 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
         <v>6</v>
       </c>
-      <c r="F2" s="1">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
         <v>8.5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <v>8.5</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
         <v>8.5</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -703,51 +756,71 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="9"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="1">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -755,29 +828,42 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="2">
-        <f>SUM(D2:D12)</f>
-        <v>62.5</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4">
-        <f>SUM(F2:F12)</f>
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="2">
+        <f>SUM(E2:E13)</f>
+        <v>74.5</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4">
+        <f>SUM(G2:G13)</f>
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{D4215E3C-901B-458D-9754-A4303D9EF53F}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{A7B12602-16F5-46EB-A0EF-0B325406AD2B}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{4BF2CE28-0012-4D71-BA54-E73EF547FD7A}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{9263DD53-D4E2-49E7-A600-2B944D5013C6}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{D4215E3C-901B-458D-9754-A4303D9EF53F}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{A7B12602-16F5-46EB-A0EF-0B325406AD2B}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{4BF2CE28-0012-4D71-BA54-E73EF547FD7A}"/>
+    <hyperlink ref="H2" r:id="rId4" xr:uid="{9263DD53-D4E2-49E7-A600-2B944D5013C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Altium project and excel documents
</commit_message>
<xml_diff>
--- a/ETRX_FECU/HW_FECU.xlsx
+++ b/ETRX_FECU/HW_FECU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9068b3d81be815ab/download/New/download/Documentos/GitHub/ADCAN/ETRX_FECU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_AD4D2F04E46CFB4ACB3E201215D3DB9A693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A222F48-7E7F-4AF4-BD4B-269E721E1390}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="11_AD4D2F04E46CFB4ACB3E201215D3DB9A693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86220E34-13F2-45C7-8BA4-7B51A45B9865}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="3150" windowWidth="18780" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Sensor</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Susp_F_R</t>
   </si>
   <si>
-    <t>Front_Alive</t>
-  </si>
-  <si>
     <t>Shutdown_Setas</t>
   </si>
   <si>
@@ -132,15 +129,24 @@
   </si>
   <si>
     <t>P (W)</t>
+  </si>
+  <si>
+    <t>Emergency button</t>
+  </si>
+  <si>
+    <t>Expansion_GPIO</t>
+  </si>
+  <si>
+    <t>Expansion_COMs</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -285,7 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -304,6 +309,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,16 +606,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>2</v>
@@ -622,7 +631,10 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <f>C2*(E2/1000)</f>
+        <v>0.18</v>
+      </c>
       <c r="E2" s="1">
         <v>36</v>
       </c>
@@ -633,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -646,7 +658,10 @@
       <c r="C3" s="1">
         <v>5</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D15" si="0">C3*(E3/1000)</f>
+        <v>4.2500000000000003E-2</v>
+      </c>
       <c r="E3" s="1">
         <v>8.5</v>
       </c>
@@ -657,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -670,7 +685,10 @@
       <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2500000000000003E-2</v>
+      </c>
       <c r="E4" s="1">
         <v>8.5</v>
       </c>
@@ -681,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -694,7 +712,10 @@
       <c r="C5" s="1">
         <v>5</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2500000000000003E-2</v>
+      </c>
       <c r="E5" s="1">
         <v>8.5</v>
       </c>
@@ -705,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -713,17 +734,22 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -731,130 +757,215 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
         <v>24</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>3.3</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="1">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>5</v>
       </c>
       <c r="G9" s="1">
-        <v>4</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1">
-        <v>2</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9599999999999996E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="2">
-        <f>SUM(E2:E13)</f>
-        <v>74.5</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4">
-        <f>SUM(G2:G13)</f>
-        <v>21</v>
-      </c>
-      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3E-3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3E-3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="2">
+        <f>SUM(E2:E15)</f>
+        <v>75.5</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4">
+        <f>SUM(G2:G15)</f>
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>